<commit_message>
feat: get total sum UZS
</commit_message>
<xml_diff>
--- a/invoice_january.xlsx
+++ b/invoice_january.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,32 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>45</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Product 2</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>32000.00</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>45687.78773686659</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>192000.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>